<commit_message>
85101 - refactored as both reports are similar in many ways.
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.Operations.Reports.Reports/Templates/ILRFileSubmissionPerDayReport.xlsx
+++ b/src/ESFA.DC.Operations.Reports.Reports/Templates/ILRFileSubmissionPerDayReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSTS\DCT\DC-Operations-Reports\src\ESFA.DC.Operations.Reports.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329F0414-77E1-4776-802A-DB228814ABBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0411FCBA-AEAA-4108-9A0E-D635A21F2BCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5F8E5E8B-81CE-49AB-8EE1-D1C01E6C85E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5F8E5E8B-81CE-49AB-8EE1-D1C01E6C85E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart - ILR File Submissions pe" sheetId="2" r:id="rId1"/>
@@ -33,16 +33,16 @@
     <t>&amp;=IlrSubmissionsInfoInfo.ReportTitle</t>
   </si>
   <si>
-    <t>&amp;=IlrSubmissionsInfo.IlrFileSubmissionsPerDayList.NumberOfSubmissions</t>
-  </si>
-  <si>
     <t>&amp;=IlrSubmissionsInfo.Period</t>
   </si>
   <si>
-    <t>&amp;=IlrSubmissionsInfo.IlrFileSubmissionsPerDayList.DaysToClose</t>
+    <t>&amp;=IlrSubmissionsInfo.ChartTitle</t>
   </si>
   <si>
-    <t>&amp;=IlrSubmissionsInfo.ChartTitle</t>
+    <t>&amp;=IlrSubmissionsInfo.SubmissionsPerDayList.NumberOfSubmissions</t>
+  </si>
+  <si>
+    <t>&amp;=IlrSubmissionsInfo.SubmissionsPerDayList.DaysToClose</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>&amp;=IlrSubmissionsInfo.IlrFileSubmissionsPerDayList.DaysToClose</c:v>
+                  <c:v>&amp;=IlrSubmissionsInfo.SubmissionsPerDayList.DaysToClose</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1605,7 +1605,7 @@
   <dimension ref="C26:W92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,7 +1644,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="V31" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="3:22" ht="25.5" x14ac:dyDescent="0.25">
@@ -1676,15 +1676,15 @@
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>